<commit_message>
Add support for updating custom rules
</commit_message>
<xml_diff>
--- a/frontend/public/custom-rules-template.xlsx
+++ b/frontend/public/custom-rules-template.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
   <si>
     <t>Ext Number</t>
   </si>
@@ -68,7 +68,7 @@
     <t>Transfer Extension</t>
   </si>
   <si>
-    <t>Extermal Number</t>
+    <t>External Number</t>
   </si>
   <si>
     <t>Voicemail Recipient</t>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>After Hours</t>
+  </si>
+  <si>
+    <t>132129685272</t>
   </si>
   <si>
     <t>321-648-3694</t>
@@ -1053,7 +1056,7 @@
       <c r="T23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="4"/>
+      <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1075,7 +1078,7 @@
       <c r="T24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1097,7 +1100,7 @@
       <c r="T25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="4"/>
+      <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1119,7 +1122,7 @@
       <c r="T26" s="4"/>
     </row>
     <row r="27">
-      <c r="A27" s="4"/>
+      <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1141,7 +1144,7 @@
       <c r="T27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="4"/>
+      <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1163,7 +1166,7 @@
       <c r="T28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="4"/>
+      <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1185,7 +1188,7 @@
       <c r="T29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="4"/>
+      <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1207,7 +1210,7 @@
       <c r="T30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="4"/>
+      <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -1229,7 +1232,7 @@
       <c r="T31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="4"/>
+      <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -1251,7 +1254,7 @@
       <c r="T32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="4"/>
+      <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -1273,7 +1276,7 @@
       <c r="T33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="4"/>
+      <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1295,7 +1298,7 @@
       <c r="T34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="4"/>
+      <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -1317,7 +1320,7 @@
       <c r="T35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="4"/>
+      <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1339,7 +1342,7 @@
       <c r="T36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="4"/>
+      <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -1361,7 +1364,7 @@
       <c r="T37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="4"/>
+      <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -1383,7 +1386,7 @@
       <c r="T38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="4"/>
+      <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -1405,7 +1408,7 @@
       <c r="T39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="4"/>
+      <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -1427,7 +1430,7 @@
       <c r="T40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="4"/>
+      <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -1449,7 +1452,7 @@
       <c r="T41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="4"/>
+      <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -1471,7 +1474,7 @@
       <c r="T42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="4"/>
+      <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -1493,7 +1496,7 @@
       <c r="T43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="4"/>
+      <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -1515,7 +1518,7 @@
       <c r="T44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="4"/>
+      <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -1537,7 +1540,7 @@
       <c r="T45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="4"/>
+      <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -1559,7 +1562,7 @@
       <c r="T46" s="4"/>
     </row>
     <row r="47">
-      <c r="A47" s="4"/>
+      <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -1581,7 +1584,7 @@
       <c r="T47" s="4"/>
     </row>
     <row r="48">
-      <c r="A48" s="4"/>
+      <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -1603,7 +1606,7 @@
       <c r="T48" s="4"/>
     </row>
     <row r="49">
-      <c r="A49" s="4"/>
+      <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -1625,7 +1628,7 @@
       <c r="T49" s="4"/>
     </row>
     <row r="50">
-      <c r="A50" s="4"/>
+      <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -1647,7 +1650,7 @@
       <c r="T50" s="4"/>
     </row>
     <row r="51">
-      <c r="A51" s="4"/>
+      <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
@@ -1669,7 +1672,7 @@
       <c r="T51" s="4"/>
     </row>
     <row r="52">
-      <c r="A52" s="4"/>
+      <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -1691,7 +1694,7 @@
       <c r="T52" s="4"/>
     </row>
     <row r="53">
-      <c r="A53" s="4"/>
+      <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -1713,7 +1716,7 @@
       <c r="T53" s="4"/>
     </row>
     <row r="54">
-      <c r="A54" s="4"/>
+      <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -1735,7 +1738,7 @@
       <c r="T54" s="4"/>
     </row>
     <row r="55">
-      <c r="A55" s="4"/>
+      <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -1757,7 +1760,7 @@
       <c r="T55" s="4"/>
     </row>
     <row r="56">
-      <c r="A56" s="4"/>
+      <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -1779,7 +1782,7 @@
       <c r="T56" s="4"/>
     </row>
     <row r="57">
-      <c r="A57" s="4"/>
+      <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -1801,7 +1804,7 @@
       <c r="T57" s="4"/>
     </row>
     <row r="58">
-      <c r="A58" s="4"/>
+      <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -1823,7 +1826,7 @@
       <c r="T58" s="4"/>
     </row>
     <row r="59">
-      <c r="A59" s="4"/>
+      <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -1845,7 +1848,7 @@
       <c r="T59" s="4"/>
     </row>
     <row r="60">
-      <c r="A60" s="4"/>
+      <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -1867,7 +1870,7 @@
       <c r="T60" s="4"/>
     </row>
     <row r="61">
-      <c r="A61" s="4"/>
+      <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -1889,7 +1892,7 @@
       <c r="T61" s="4"/>
     </row>
     <row r="62">
-      <c r="A62" s="4"/>
+      <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -1911,7 +1914,7 @@
       <c r="T62" s="4"/>
     </row>
     <row r="63">
-      <c r="A63" s="4"/>
+      <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
@@ -1933,7 +1936,7 @@
       <c r="T63" s="4"/>
     </row>
     <row r="64">
-      <c r="A64" s="4"/>
+      <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -1955,7 +1958,7 @@
       <c r="T64" s="4"/>
     </row>
     <row r="65">
-      <c r="A65" s="4"/>
+      <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
@@ -1977,7 +1980,7 @@
       <c r="T65" s="4"/>
     </row>
     <row r="66">
-      <c r="A66" s="4"/>
+      <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -1999,7 +2002,7 @@
       <c r="T66" s="4"/>
     </row>
     <row r="67">
-      <c r="A67" s="4"/>
+      <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -2021,7 +2024,7 @@
       <c r="T67" s="4"/>
     </row>
     <row r="68">
-      <c r="A68" s="4"/>
+      <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -2043,7 +2046,7 @@
       <c r="T68" s="4"/>
     </row>
     <row r="69">
-      <c r="A69" s="4"/>
+      <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
@@ -2065,7 +2068,7 @@
       <c r="T69" s="4"/>
     </row>
     <row r="70">
-      <c r="A70" s="4"/>
+      <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
@@ -2087,7 +2090,7 @@
       <c r="T70" s="4"/>
     </row>
     <row r="71">
-      <c r="A71" s="4"/>
+      <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
@@ -2109,7 +2112,7 @@
       <c r="T71" s="4"/>
     </row>
     <row r="72">
-      <c r="A72" s="4"/>
+      <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
@@ -2131,7 +2134,7 @@
       <c r="T72" s="4"/>
     </row>
     <row r="73">
-      <c r="A73" s="4"/>
+      <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -2153,7 +2156,7 @@
       <c r="T73" s="4"/>
     </row>
     <row r="74">
-      <c r="A74" s="4"/>
+      <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -2175,7 +2178,7 @@
       <c r="T74" s="4"/>
     </row>
     <row r="75">
-      <c r="A75" s="4"/>
+      <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
@@ -2197,7 +2200,7 @@
       <c r="T75" s="4"/>
     </row>
     <row r="76">
-      <c r="A76" s="4"/>
+      <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -22570,7 +22573,8 @@
     <col customWidth="1" min="3" max="3" width="16.38"/>
     <col customWidth="1" min="4" max="6" width="12.63"/>
     <col customWidth="1" min="7" max="7" width="21.38"/>
-    <col customWidth="1" min="8" max="15" width="15.75"/>
+    <col customWidth="1" min="8" max="8" width="17.0"/>
+    <col customWidth="1" min="9" max="15" width="15.75"/>
     <col customWidth="1" min="16" max="16" width="20.88"/>
     <col customWidth="1" min="17" max="17" width="18.63"/>
     <col customWidth="1" min="18" max="19" width="23.88"/>
@@ -22894,7 +22898,9 @@
         <v>28</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H9" s="3" t="s">
         <v>40</v>
       </c>
@@ -22911,7 +22917,7 @@
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T9" s="4"/>
     </row>

</xml_diff>